<commit_message>
Added content to ch3, a fastcluster vs naive graph, and reorganized a little of the parallel section
</commit_message>
<xml_diff>
--- a/results/BinningTimes.xlsx
+++ b/results/BinningTimes.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="0" windowWidth="27880" windowHeight="16960" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Fastcluster" sheetId="3" r:id="rId3"/>
+    <sheet name="fastvsDan" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="timed" localSheetId="0">Sheet1!$C$5:$H$55</definedName>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="94">
   <si>
     <t>100.fa</t>
   </si>
@@ -334,6 +335,12 @@
   </si>
   <si>
     <t>sequences</t>
+  </si>
+  <si>
+    <t>FastClust</t>
+  </si>
+  <si>
+    <t>Danny</t>
   </si>
 </sst>
 </file>
@@ -382,8 +389,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -400,19 +425,37 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -822,11 +865,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2060344216"/>
-        <c:axId val="2060349480"/>
+        <c:axId val="2099307816"/>
+        <c:axId val="2099302536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2060344216"/>
+        <c:axId val="2099307816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +897,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060349480"/>
+        <c:crossAx val="2099302536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -862,7 +905,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2060349480"/>
+        <c:axId val="2099302536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,7 +935,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060344216"/>
+        <c:crossAx val="2099307816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1299,11 +1342,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2060425368"/>
-        <c:axId val="2060430744"/>
+        <c:axId val="2101514760"/>
+        <c:axId val="2101520136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2060425368"/>
+        <c:axId val="2101514760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1332,7 +1375,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060430744"/>
+        <c:crossAx val="2101520136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1340,7 +1383,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2060430744"/>
+        <c:axId val="2101520136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1370,7 +1413,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060425368"/>
+        <c:crossAx val="2101514760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1421,7 +1464,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1495,11 +1537,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2060875304"/>
-        <c:axId val="2056269528"/>
+        <c:axId val="2101562392"/>
+        <c:axId val="2101565288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2060875304"/>
+        <c:axId val="2101562392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,12 +1551,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056269528"/>
+        <c:crossAx val="2101565288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2056269528"/>
+        <c:axId val="2101565288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,14 +1567,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060875304"/>
+        <c:crossAx val="2101562392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1836,11 +1877,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2049015496"/>
-        <c:axId val="2049001080"/>
+        <c:axId val="2101606360"/>
+        <c:axId val="2101609240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2049015496"/>
+        <c:axId val="2101606360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1850,7 +1891,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049001080"/>
+        <c:crossAx val="2101609240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1858,7 +1899,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2049001080"/>
+        <c:axId val="2101609240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1888,7 +1929,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049015496"/>
+        <c:crossAx val="2101606360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2194,11 +2235,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2048983864"/>
-        <c:axId val="2033002760"/>
+        <c:axId val="2101642152"/>
+        <c:axId val="2101645032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2048983864"/>
+        <c:axId val="2101642152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2208,7 +2249,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2033002760"/>
+        <c:crossAx val="2101645032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2216,7 +2257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2033002760"/>
+        <c:axId val="2101645032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2246,9 +2287,582 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2048983864"/>
+        <c:crossAx val="2101642152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Clustering Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Naive</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fastvsDan!$H$6:$H$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>650.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>850.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>950.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1050.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1100.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1150.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1300.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1350.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1400.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1450.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1550.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1650.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1700.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1800.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1850.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1900.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1950.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2050.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2150.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2250.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2350.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2450.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fastvsDan!$I$6:$I$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.0427350997925</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0791380405426</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.161091804504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.326465845108</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.502826929092</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.839502096176</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.30766487122</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.08065605164</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.80596494675</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.74241018295</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.80630707741</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.82297301292</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.4605147839</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.5182950497</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.3748860359</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21.7473368645</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29.195939064</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>33.6614921093</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>34.4277360439</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37.7517681122</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>49.4680361748</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>56.7790288925</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>66.95442581179999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>63.911960125</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>85.945950985</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>97.332930088</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>109.984098911</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>107.176070929</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>136.803373814</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>151.426113844</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>168.614411116</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>151.93026495</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>201.425773859</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>219.556095839</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>240.297363997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>228.134633064</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>284.68508482</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>305.243964195</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>310.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>330.047247887</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>411.710768938</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>449.603285074</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>449.938149929</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>425.385893106</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>546.542893887</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>572.582892895</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>590.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>600.293020964</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>741.14845705</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>806.123780966</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>fastcluster</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fastvsDan!$D$6:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8500.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fastvsDan!$E$6:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>26.39135098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.32804084</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.80671215</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.47904706</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.39954281</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>114.8739121</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>139.980346</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>172.9268301</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>204.3303971</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>244.4220428</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>286.8578129</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>347.793083</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400.543118</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>487.4467471</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2133599816"/>
+        <c:axId val="2134331016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2133599816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Sequences</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2134331016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2134331016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>completion (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2133599816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -2420,6 +3034,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2764,8 +3413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3347,6 +3996,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3481,8 +4131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4060,4 +4710,1207 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D4:J55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="4" spans="4:10">
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10">
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10">
+      <c r="D6">
+        <v>2500</v>
+      </c>
+      <c r="E6">
+        <v>26.391350979999999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>28</v>
+      </c>
+      <c r="H6">
+        <f>J6/2</f>
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>4.2735099792500002E-2</v>
+      </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10">
+      <c r="D7">
+        <v>3000</v>
+      </c>
+      <c r="E7">
+        <v>35.32804084</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>44</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H55" si="0">J7/2</f>
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>7.9138040542599999E-2</v>
+      </c>
+      <c r="J7">
+        <f>J6+100</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10">
+      <c r="D8">
+        <v>3500</v>
+      </c>
+      <c r="E8">
+        <v>49.806712150000003</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>51</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="I8">
+        <v>0.16109180450400001</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J55" si="1">J7+100</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10">
+      <c r="D9">
+        <v>4000</v>
+      </c>
+      <c r="E9">
+        <v>69.479047059999999</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>66</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="I9">
+        <v>0.32646584510799997</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10">
+      <c r="D10">
+        <v>4500</v>
+      </c>
+      <c r="E10">
+        <v>90.39954281</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>74</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="I10">
+        <v>0.502826929092</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10">
+      <c r="D11">
+        <v>5000</v>
+      </c>
+      <c r="E11">
+        <v>114.8739121</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>84</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="I11">
+        <v>0.83950209617600002</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10">
+      <c r="D12">
+        <v>5500</v>
+      </c>
+      <c r="E12">
+        <v>139.980346</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>92</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="I12">
+        <v>1.3076648712200001</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10">
+      <c r="D13">
+        <v>6000</v>
+      </c>
+      <c r="E13">
+        <v>172.92683009999999</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="I13">
+        <v>2.0806560516400001</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10">
+      <c r="D14">
+        <v>6500</v>
+      </c>
+      <c r="E14">
+        <v>204.3303971</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <v>106</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+      <c r="I14">
+        <v>2.8059649467500001</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10">
+      <c r="D15">
+        <v>7000</v>
+      </c>
+      <c r="E15">
+        <v>244.42204280000001</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>115</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="I15">
+        <v>3.7424101829500001</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10">
+      <c r="D16">
+        <v>7500</v>
+      </c>
+      <c r="E16">
+        <v>286.8578129</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16">
+        <v>125</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>550</v>
+      </c>
+      <c r="I16">
+        <v>6.8063070774099996</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10">
+      <c r="D17">
+        <v>8000</v>
+      </c>
+      <c r="E17">
+        <v>347.79308300000002</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17">
+        <v>131</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="I17">
+        <v>6.8229730129200004</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10">
+      <c r="D18">
+        <v>8500</v>
+      </c>
+      <c r="E18">
+        <v>400.54311799999999</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18">
+        <v>137</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>650</v>
+      </c>
+      <c r="I18">
+        <v>10.460514783900001</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10">
+      <c r="D19">
+        <v>9000</v>
+      </c>
+      <c r="E19">
+        <v>487.44674709999998</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <v>145</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="I19">
+        <v>12.518295049700001</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10">
+      <c r="D20">
+        <v>9500</v>
+      </c>
+      <c r="E20">
+        <v>617.7057221</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20">
+        <v>149</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+      <c r="I20">
+        <v>17.374886035900001</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10">
+      <c r="D21">
+        <v>10000</v>
+      </c>
+      <c r="E21">
+        <v>637.98285390000001</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <v>156</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="I21">
+        <v>21.747336864499999</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10">
+      <c r="D22">
+        <v>10500</v>
+      </c>
+      <c r="E22">
+        <v>647.26994609999997</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22">
+        <v>161</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>850</v>
+      </c>
+      <c r="I22">
+        <v>29.195939064000001</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10">
+      <c r="D23">
+        <v>11000</v>
+      </c>
+      <c r="E23">
+        <v>695.14443400000005</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23">
+        <v>172</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="I23">
+        <v>33.661492109299999</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10">
+      <c r="D24">
+        <v>11500</v>
+      </c>
+      <c r="E24">
+        <v>770.0483921</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24">
+        <v>179</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>950</v>
+      </c>
+      <c r="I24">
+        <v>34.427736043899998</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10">
+      <c r="D25">
+        <v>12000</v>
+      </c>
+      <c r="E25">
+        <v>837.06177690000004</v>
+      </c>
+      <c r="F25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25">
+        <v>184</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="I25">
+        <v>37.751768112199997</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10">
+      <c r="D26">
+        <v>12500</v>
+      </c>
+      <c r="E26">
+        <v>901.887742</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26">
+        <v>189</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>1050</v>
+      </c>
+      <c r="I26">
+        <v>49.468036174799998</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10">
+      <c r="D27">
+        <v>13000</v>
+      </c>
+      <c r="E27">
+        <v>935.25518199999999</v>
+      </c>
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27">
+        <v>194</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="I27">
+        <v>56.779028892500001</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10">
+      <c r="D28">
+        <v>13500</v>
+      </c>
+      <c r="E28">
+        <v>1022.329304</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28">
+        <v>202</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>1150</v>
+      </c>
+      <c r="I28">
+        <v>66.954425811799993</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="29" spans="4:10">
+      <c r="D29">
+        <v>14000</v>
+      </c>
+      <c r="E29">
+        <v>1108.219955</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29">
+        <v>208</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="I29">
+        <v>63.911960125</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="30" spans="4:10">
+      <c r="D30">
+        <v>14500</v>
+      </c>
+      <c r="E30">
+        <v>1170.302727</v>
+      </c>
+      <c r="F30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30">
+        <v>212</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
+      <c r="I30">
+        <v>85.945950984999996</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="31" spans="4:10">
+      <c r="D31">
+        <v>15000</v>
+      </c>
+      <c r="E31">
+        <v>1285.311909</v>
+      </c>
+      <c r="F31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31">
+        <v>215</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>1300</v>
+      </c>
+      <c r="I31">
+        <v>97.332930087999998</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="32" spans="4:10">
+      <c r="D32">
+        <v>15500</v>
+      </c>
+      <c r="E32">
+        <v>1341.4548</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32">
+        <v>222</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>1350</v>
+      </c>
+      <c r="I32">
+        <v>109.984098911</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="33" spans="4:10">
+      <c r="D33">
+        <v>16000</v>
+      </c>
+      <c r="E33">
+        <v>1348.172313</v>
+      </c>
+      <c r="F33" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33">
+        <v>226</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>1400</v>
+      </c>
+      <c r="I33">
+        <v>107.17607092900001</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="34" spans="4:10">
+      <c r="D34">
+        <v>16500</v>
+      </c>
+      <c r="E34">
+        <v>1511.0778270000001</v>
+      </c>
+      <c r="F34" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34">
+        <v>233</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>1450</v>
+      </c>
+      <c r="I34">
+        <v>136.803373814</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="35" spans="4:10">
+      <c r="D35">
+        <v>17000</v>
+      </c>
+      <c r="E35">
+        <v>1596.9462880000001</v>
+      </c>
+      <c r="F35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35">
+        <v>235</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="I35">
+        <v>151.42611384400001</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="36" spans="4:10">
+      <c r="D36">
+        <v>17500</v>
+      </c>
+      <c r="E36">
+        <v>1679.106994</v>
+      </c>
+      <c r="F36" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36">
+        <v>240</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>1550</v>
+      </c>
+      <c r="I36">
+        <v>168.61441111600001</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="37" spans="4:10">
+      <c r="D37">
+        <v>18000</v>
+      </c>
+      <c r="E37">
+        <v>1818.3896099999999</v>
+      </c>
+      <c r="F37" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37">
+        <v>268</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+      <c r="I37">
+        <v>151.93026495000001</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="38" spans="4:10">
+      <c r="D38">
+        <v>18500</v>
+      </c>
+      <c r="E38">
+        <v>2008.285748</v>
+      </c>
+      <c r="F38" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38">
+        <v>281</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>1650</v>
+      </c>
+      <c r="I38">
+        <v>201.425773859</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="39" spans="4:10">
+      <c r="D39">
+        <v>19000</v>
+      </c>
+      <c r="E39">
+        <v>2577.8576429999998</v>
+      </c>
+      <c r="F39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G39">
+        <v>302</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="I39">
+        <v>219.55609583899999</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="40" spans="4:10">
+      <c r="F40" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40">
+        <v>317</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>1750</v>
+      </c>
+      <c r="I40">
+        <v>240.29736399699999</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="41" spans="4:10">
+      <c r="F41" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41">
+        <v>328</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+      <c r="I41">
+        <v>228.13463306400001</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="1"/>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="42" spans="4:10">
+      <c r="F42" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42">
+        <v>341</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>1850</v>
+      </c>
+      <c r="I42">
+        <v>284.68508481999999</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="1"/>
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="43" spans="4:10">
+      <c r="F43" t="s">
+        <v>37</v>
+      </c>
+      <c r="G43">
+        <v>355</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>1900</v>
+      </c>
+      <c r="I43">
+        <v>305.24396419499999</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="44" spans="4:10">
+      <c r="F44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G44">
+        <v>368</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>1950</v>
+      </c>
+      <c r="I44">
+        <v>310</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="1"/>
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="45" spans="4:10">
+      <c r="F45" t="s">
+        <v>39</v>
+      </c>
+      <c r="G45">
+        <v>379</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="I45">
+        <v>330.04724788700003</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="46" spans="4:10">
+      <c r="F46" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46">
+        <v>389</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+      <c r="I46">
+        <v>411.710768938</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="1"/>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="47" spans="4:10">
+      <c r="F47" t="s">
+        <v>41</v>
+      </c>
+      <c r="G47">
+        <v>397</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="I47">
+        <v>449.60328507399998</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="1"/>
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="48" spans="4:10">
+      <c r="F48" t="s">
+        <v>42</v>
+      </c>
+      <c r="G48">
+        <v>409</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="0"/>
+        <v>2150</v>
+      </c>
+      <c r="I48">
+        <v>449.93814992900002</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="1"/>
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="49" spans="6:10">
+      <c r="F49" t="s">
+        <v>43</v>
+      </c>
+      <c r="G49">
+        <v>418</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+      <c r="I49">
+        <v>425.38589310600003</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="1"/>
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="50" spans="6:10">
+      <c r="F50" t="s">
+        <v>44</v>
+      </c>
+      <c r="G50">
+        <v>428</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="0"/>
+        <v>2250</v>
+      </c>
+      <c r="I50">
+        <v>546.54289388699999</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="1"/>
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="51" spans="6:10">
+      <c r="F51" t="s">
+        <v>45</v>
+      </c>
+      <c r="G51">
+        <v>434</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+      <c r="I51">
+        <v>572.58289289499999</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="1"/>
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="52" spans="6:10">
+      <c r="F52" t="s">
+        <v>46</v>
+      </c>
+      <c r="G52">
+        <v>445</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="0"/>
+        <v>2350</v>
+      </c>
+      <c r="I52">
+        <v>590</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="1"/>
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="53" spans="6:10">
+      <c r="F53" t="s">
+        <v>47</v>
+      </c>
+      <c r="G53">
+        <v>452</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="I53">
+        <v>600.29302096399999</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="1"/>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="54" spans="6:10">
+      <c r="F54" t="s">
+        <v>48</v>
+      </c>
+      <c r="G54">
+        <v>461</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="0"/>
+        <v>2450</v>
+      </c>
+      <c r="I54">
+        <v>741.14845705000005</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="1"/>
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="55" spans="6:10">
+      <c r="F55" t="s">
+        <v>49</v>
+      </c>
+      <c r="G55">
+        <v>476</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="I55">
+        <v>806.12378096600003</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
last changes for the night, broke 38 pages, tomorrow should hit 40 page mark
</commit_message>
<xml_diff>
--- a/results/BinningTimes.xlsx
+++ b/results/BinningTimes.xlsx
@@ -2869,6 +2869,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -3052,10 +3057,10 @@
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>

<commit_message>
Added hundred rep ES1vES2 results to appendix and made a few cleanups
</commit_message>
<xml_diff>
--- a/results/BinningTimes.xlsx
+++ b/results/BinningTimes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13840" yWindow="4280" windowWidth="22200" windowHeight="16140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -493,6 +493,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -516,6 +517,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -863,11 +865,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2051355320"/>
-        <c:axId val="2051360632"/>
+        <c:axId val="2102058600"/>
+        <c:axId val="2102063864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2051355320"/>
+        <c:axId val="2102058600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,12 +891,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2051360632"/>
+        <c:crossAx val="2102063864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -902,7 +905,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2051360632"/>
+        <c:axId val="2102063864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -925,13 +928,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2051355320"/>
+        <c:crossAx val="2102058600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -983,6 +987,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1003,6 +1008,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1336,11 +1342,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2051442552"/>
-        <c:axId val="2051447928"/>
+        <c:axId val="2102098072"/>
+        <c:axId val="2102103448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2051442552"/>
+        <c:axId val="2102098072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,13 +1368,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2051447928"/>
+        <c:crossAx val="2102103448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1376,7 +1383,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2051447928"/>
+        <c:axId val="2102103448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1399,13 +1406,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2051442552"/>
+        <c:crossAx val="2102098072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1456,6 +1464,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1529,11 +1538,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2050229368"/>
-        <c:axId val="2050232264"/>
+        <c:axId val="2102146664"/>
+        <c:axId val="2102149560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2050229368"/>
+        <c:axId val="2102146664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1543,12 +1552,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2050232264"/>
+        <c:crossAx val="2102149560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2050232264"/>
+        <c:axId val="2102149560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,13 +1568,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2050229368"/>
+        <c:crossAx val="2102146664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1610,6 +1620,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1630,6 +1641,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1867,11 +1879,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2050247016"/>
-        <c:axId val="2050249896"/>
+        <c:axId val="2102191064"/>
+        <c:axId val="2102193944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2050247016"/>
+        <c:axId val="2102191064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1881,7 +1893,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2050249896"/>
+        <c:crossAx val="2102193944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1889,7 +1901,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2050249896"/>
+        <c:axId val="2102193944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,13 +1924,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2050247016"/>
+        <c:crossAx val="2102191064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1965,6 +1978,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1985,6 +1999,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2222,11 +2237,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2050286296"/>
-        <c:axId val="2050289176"/>
+        <c:axId val="2102226904"/>
+        <c:axId val="2102229784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2050286296"/>
+        <c:axId val="2102226904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2236,7 +2251,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2050289176"/>
+        <c:crossAx val="2102229784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2244,7 +2259,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2050289176"/>
+        <c:axId val="2102229784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2267,13 +2282,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2050286296"/>
+        <c:crossAx val="2102226904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2780,11 +2796,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2050340984"/>
-        <c:axId val="2050346488"/>
+        <c:axId val="2102274712"/>
+        <c:axId val="2102280488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2050340984"/>
+        <c:axId val="2102274712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9000.0"/>
@@ -2819,12 +2835,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2050346488"/>
+        <c:crossAx val="2102280488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2050346488"/>
+        <c:axId val="2102280488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800.0"/>
@@ -2854,7 +2870,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2050340984"/>
+        <c:crossAx val="2102274712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3426,7 +3442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:E55"/>
     </sheetView>
   </sheetViews>
@@ -4729,7 +4745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7:H55"/>
     </sheetView>
   </sheetViews>

</xml_diff>